<commit_message>
dict is functionally correct
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_analysis.xlsx
+++ b/sp500-historical-components-and-changes/sp500_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED78B6C-6FC8-44A4-A73E-3BE20E57A7AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD59F45-FC84-4D18-B014-515F3F6883E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regular_add" sheetId="1" r:id="rId1"/>
@@ -446,10 +446,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="17.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>42811</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42814</v>
+      </c>
+      <c r="C2">
+        <v>0.2299919128417969</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>42902</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C3">
+        <v>4.9699935913085938</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>42993</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>43175</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43178</v>
+      </c>
+      <c r="C5">
+        <v>3.4099960327148442</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>43266</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43269</v>
+      </c>
+      <c r="C6">
+        <v>-1.1699981689453121</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>43455</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43458</v>
+      </c>
+      <c r="C7">
+        <v>-1.819999694824219</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>43728</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43731</v>
+      </c>
+      <c r="C8">
+        <v>-0.7400054931640625</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>43819</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43822</v>
+      </c>
+      <c r="C9">
+        <v>0.80999755859375</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -478,22 +649,28 @@
       <c r="A2" s="2">
         <v>42811</v>
       </c>
+      <c r="B2" s="3">
+        <v>42814</v>
+      </c>
       <c r="C2">
-        <v>0.2299919128417969</v>
+        <v>-0.35999870300292969</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>42902</v>
       </c>
+      <c r="B3" s="3">
+        <v>42905</v>
+      </c>
       <c r="C3">
-        <v>4.9699935913085938</v>
+        <v>-7.9999923706054688E-2</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -504,293 +681,70 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
-        <v>42978</v>
+        <v>43175</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43178</v>
+      </c>
+      <c r="C4">
+        <v>0.64000034332275391</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
-        <v>42993</v>
+        <v>43266</v>
       </c>
       <c r="B5" s="3">
-        <v>42996</v>
+        <v>43269</v>
       </c>
       <c r="C5">
-        <v>0.25</v>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
-        <v>43175</v>
+        <v>43455</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43458</v>
       </c>
       <c r="C6">
-        <v>3.4099960327148442</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
-        <v>43266</v>
+        <v>43819</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43822</v>
       </c>
       <c r="C7">
-        <v>-1.1699981689453121</v>
+        <v>-1.0800018310546879</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2">
-        <v>43455</v>
-      </c>
-      <c r="C8">
-        <v>-1.819999694824219</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2">
-        <v>43728</v>
-      </c>
-      <c r="B10" s="3">
-        <v>43731</v>
-      </c>
-      <c r="C10">
-        <v>-0.7400054931640625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2">
-        <v>43819</v>
-      </c>
-      <c r="C11">
-        <v>0.80999755859375</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="2" width="17.41796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2">
-        <v>42809</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2">
-        <v>42811</v>
-      </c>
-      <c r="B3" s="3">
-        <v>42814</v>
-      </c>
-      <c r="C3">
-        <v>-0.35999870300292969</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2">
-        <v>42887</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2">
-        <v>42902</v>
-      </c>
-      <c r="B5" s="3">
-        <v>42905</v>
-      </c>
-      <c r="C5">
-        <v>-7.9999923706054688E-2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2">
-        <v>43165</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2">
-        <v>43175</v>
-      </c>
-      <c r="B7" s="3">
-        <v>43178</v>
-      </c>
-      <c r="C7">
-        <v>0.64000034332275391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2">
-        <v>43257</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2">
-        <v>43266</v>
-      </c>
-      <c r="B9" s="3">
-        <v>43269</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2">
-        <v>43434</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2">
-        <v>43455</v>
-      </c>
-      <c r="B11" s="3">
-        <v>43458</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2">
-        <v>43805</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2">
-        <v>43819</v>
-      </c>
-      <c r="B13" s="3">
-        <v>43822</v>
-      </c>
-      <c r="C13">
-        <v>-1.0800018310546879</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -800,16 +754,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView topLeftCell="A42" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="2" width="17.41796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
@@ -832,6 +781,9 @@
       <c r="A2" s="2">
         <v>42373</v>
       </c>
+      <c r="B2" s="3">
+        <v>42374</v>
+      </c>
       <c r="C2">
         <v>-3.6821136474609379</v>
       </c>
@@ -853,7 +805,7 @@
         <v>-1.19000244140625</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -904,7 +856,7 @@
         <v>-0.8600006103515625</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -920,11 +872,20 @@
       <c r="C7">
         <v>-1.7700004577636721</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>42458</v>
       </c>
+      <c r="B8" s="3">
+        <v>42459</v>
+      </c>
       <c r="C8">
         <v>3.4999847412109382E-2</v>
       </c>
@@ -962,11 +923,20 @@
       <c r="C10">
         <v>-0.238311767578125</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>42475</v>
       </c>
+      <c r="B11" s="3">
+        <v>42478</v>
+      </c>
       <c r="C11">
         <v>-1.6100006103515621</v>
       </c>
@@ -981,6 +951,9 @@
       <c r="A12" s="2">
         <v>42482</v>
       </c>
+      <c r="B12" s="3">
+        <v>42485</v>
+      </c>
       <c r="C12">
         <v>-0.9799957275390625</v>
       </c>
@@ -1137,11 +1110,20 @@
       <c r="C21">
         <v>-3.170013427734375</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>42620</v>
       </c>
+      <c r="B22" s="3">
+        <v>42621</v>
+      </c>
       <c r="C22">
         <v>2.889984130859375</v>
       </c>
@@ -1163,7 +1145,7 @@
         <v>-0.230010986328125</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1180,7 +1162,7 @@
         <v>-0.73999977111816406</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1197,7 +1179,7 @@
         <v>-3.1491546630859379</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1247,11 +1229,20 @@
       <c r="C28">
         <v>-0.90999603271484375</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>42795</v>
       </c>
+      <c r="B29" s="3">
+        <v>42796</v>
+      </c>
       <c r="C29">
         <v>-1.9499969482421879</v>
       </c>
@@ -1272,16 +1263,25 @@
       <c r="C30">
         <v>-1.459999084472656</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>42809</v>
       </c>
+      <c r="B31" s="3">
+        <v>42810</v>
+      </c>
       <c r="C31">
         <v>-0.51000213623046875</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1289,7 +1289,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
-        <v>42811</v>
+        <v>42828</v>
+      </c>
+      <c r="B32" s="3">
+        <v>42829</v>
+      </c>
+      <c r="C32">
+        <v>-0.91695404052734375</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1300,13 +1306,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
-        <v>42828</v>
+        <v>42829</v>
       </c>
       <c r="B33" s="3">
-        <v>42829</v>
+        <v>42830</v>
       </c>
       <c r="C33">
-        <v>-0.91695404052734375</v>
+        <v>-0.25</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1317,32 +1323,47 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
-        <v>42829</v>
+        <v>42887</v>
       </c>
       <c r="B34" s="3">
-        <v>42830</v>
+        <v>42888</v>
       </c>
       <c r="C34">
-        <v>-0.25</v>
+        <v>0.76000213623046875</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
-        <v>42887</v>
+        <v>42941</v>
+      </c>
+      <c r="B35" s="3">
+        <v>42942</v>
       </c>
       <c r="C35">
-        <v>0.76000213623046875</v>
+        <v>-0.86999893188476563</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
-        <v>42902</v>
+        <v>42954</v>
+      </c>
+      <c r="B36" s="3">
+        <v>42955</v>
+      </c>
+      <c r="C36">
+        <v>-2.8499984741210942</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1353,27 +1374,30 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
-        <v>42941</v>
+        <v>42978</v>
       </c>
       <c r="B37" s="3">
-        <v>42942</v>
+        <v>42979</v>
       </c>
       <c r="C37">
-        <v>-0.86999893188476563</v>
+        <v>0.510009765625</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
-        <v>42954</v>
+        <v>43020</v>
+      </c>
+      <c r="B38" s="3">
+        <v>43021</v>
       </c>
       <c r="C38">
-        <v>-2.8499984741210942</v>
+        <v>6.0001373291015618E-2</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1384,13 +1408,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
-        <v>42978</v>
+        <v>43102</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43103</v>
       </c>
       <c r="C39">
-        <v>0.510009765625</v>
+        <v>-7.69000244140625</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1398,7 +1425,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
-        <v>42993</v>
+        <v>43165</v>
+      </c>
+      <c r="B40" s="3">
+        <v>43166</v>
+      </c>
+      <c r="C40">
+        <v>5.4600067138671884</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1409,16 +1442,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
-        <v>43020</v>
+        <v>43193</v>
       </c>
       <c r="B41" s="3">
-        <v>43021</v>
+        <v>43194</v>
       </c>
       <c r="C41">
-        <v>6.0001373291015618E-2</v>
+        <v>-0.2299957275390625</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1426,21 +1459,30 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
-        <v>43102</v>
+        <v>43250</v>
       </c>
       <c r="B42" s="3">
-        <v>43103</v>
+        <v>43251</v>
       </c>
       <c r="C42">
-        <v>-7.69000244140625</v>
+        <v>1.170013427734375</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
-        <v>43165</v>
+        <v>43255</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43256</v>
       </c>
       <c r="C43">
-        <v>5.4600067138671884</v>
+        <v>-1.0800018310546879</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1451,13 +1493,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
-        <v>43193</v>
+        <v>43257</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43258</v>
       </c>
       <c r="C44">
-        <v>-0.2299957275390625</v>
+        <v>0.29999923706054688</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1465,16 +1510,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
-        <v>43250</v>
+        <v>43270</v>
       </c>
       <c r="B45" s="3">
-        <v>43251</v>
+        <v>43271</v>
       </c>
       <c r="C45">
-        <v>1.170013427734375</v>
+        <v>-0.3600006103515625</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1482,24 +1527,33 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
-        <v>43255</v>
+        <v>43280</v>
       </c>
       <c r="B46" s="3">
-        <v>43256</v>
+        <v>43283</v>
       </c>
       <c r="C46">
-        <v>-1.0800018310546879</v>
+        <v>0.5500030517578125</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
-        <v>43257</v>
+        <v>43339</v>
+      </c>
+      <c r="B47" s="3">
+        <v>43340</v>
       </c>
       <c r="C47">
-        <v>0.29999923706054688</v>
+        <v>-3.78997802734375</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1507,10 +1561,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
-        <v>43266</v>
+        <v>43356</v>
+      </c>
+      <c r="B48" s="3">
+        <v>43357</v>
+      </c>
+      <c r="C48">
+        <v>-3.660003662109375</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1518,16 +1578,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
-        <v>43270</v>
+        <v>43371</v>
       </c>
       <c r="B49" s="3">
-        <v>43271</v>
+        <v>43374</v>
       </c>
       <c r="C49">
-        <v>-0.3600006103515625</v>
+        <v>0.95333099365234375</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1535,16 +1595,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
-        <v>43280</v>
+        <v>43383</v>
       </c>
       <c r="B50" s="3">
-        <v>43283</v>
+        <v>43384</v>
       </c>
       <c r="C50">
-        <v>0.5500030517578125</v>
+        <v>-2.9899978637695308</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1552,16 +1612,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
-        <v>43339</v>
+        <v>43409</v>
       </c>
       <c r="B51" s="3">
-        <v>43340</v>
+        <v>43410</v>
       </c>
       <c r="C51">
-        <v>-3.78997802734375</v>
+        <v>1.1599998474121089</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1569,41 +1629,50 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
-        <v>43356</v>
+        <v>43416</v>
       </c>
       <c r="B52" s="3">
-        <v>43357</v>
+        <v>43417</v>
       </c>
       <c r="C52">
-        <v>-3.660003662109375</v>
+        <v>-0.19000244140625</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
-        <v>43371</v>
+        <v>43434</v>
+      </c>
+      <c r="B53" s="3">
+        <v>43437</v>
       </c>
       <c r="C53">
-        <v>0.95333099365234375</v>
+        <v>-1.0800056457519529</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
-        <v>43383</v>
+        <v>43465</v>
       </c>
       <c r="B54" s="3">
-        <v>43384</v>
+        <v>43467</v>
       </c>
       <c r="C54">
-        <v>-2.9899978637695308</v>
+        <v>-1.040000915527344</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1611,21 +1680,30 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
-        <v>43409</v>
+        <v>43482</v>
       </c>
       <c r="B55" s="3">
-        <v>43410</v>
+        <v>43483</v>
       </c>
       <c r="C55">
-        <v>1.1599998474121089</v>
+        <v>6.05999755859375</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
-        <v>43416</v>
+        <v>43510</v>
+      </c>
+      <c r="B56" s="3">
+        <v>43511</v>
       </c>
       <c r="C56">
-        <v>-0.19000244140625</v>
+        <v>-0.62999725341796875</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1636,10 +1714,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
-        <v>43433</v>
+        <v>43522</v>
+      </c>
+      <c r="B57" s="3">
+        <v>43523</v>
+      </c>
+      <c r="C57">
+        <v>-4.0999984741210938</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -1647,18 +1731,30 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
-        <v>43434</v>
+        <v>43556</v>
       </c>
       <c r="B58" s="3">
-        <v>43437</v>
+        <v>43557</v>
       </c>
       <c r="C58">
-        <v>-1.0800056457519529</v>
+        <v>1.8699989318847661</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
-        <v>43455</v>
+        <v>43616</v>
+      </c>
+      <c r="B59" s="3">
+        <v>43619</v>
+      </c>
+      <c r="C59">
+        <v>-1.8299999237060549</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1669,13 +1765,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
-        <v>43465</v>
+        <v>43644</v>
       </c>
       <c r="B60" s="3">
-        <v>43467</v>
+        <v>43647</v>
       </c>
       <c r="C60">
-        <v>-1.040000915527344</v>
+        <v>5.08001708984375</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1686,38 +1782,50 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
-        <v>43482</v>
+        <v>43658</v>
       </c>
       <c r="B61" s="3">
-        <v>43483</v>
+        <v>43661</v>
       </c>
       <c r="C61">
-        <v>6.05999755859375</v>
+        <v>1.189994812011719</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
-        <v>43509</v>
+        <v>43685</v>
+      </c>
+      <c r="B62" s="3">
+        <v>43686</v>
+      </c>
+      <c r="C62">
+        <v>7.3300018310546884</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
-        <v>43510</v>
+        <v>43733</v>
       </c>
       <c r="B63" s="3">
-        <v>43511</v>
+        <v>43734</v>
       </c>
       <c r="C63">
-        <v>-0.62999725341796875</v>
+        <v>51.6201171875</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -1725,13 +1833,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
-        <v>43522</v>
+        <v>43740</v>
       </c>
       <c r="B64" s="3">
-        <v>43523</v>
+        <v>43741</v>
       </c>
       <c r="C64">
-        <v>-4.0999984741210938</v>
+        <v>-0.70999908447265625</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -1742,13 +1850,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
-        <v>43556</v>
+        <v>43789</v>
       </c>
       <c r="B65" s="3">
-        <v>43557</v>
+        <v>43790</v>
       </c>
       <c r="C65">
-        <v>1.8699989318847661</v>
+        <v>5.260009765625</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1759,16 +1867,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
-        <v>43616</v>
+        <v>43803</v>
       </c>
       <c r="B66" s="3">
-        <v>43619</v>
+        <v>43804</v>
       </c>
       <c r="C66">
-        <v>-1.8299999237060549</v>
+        <v>0.2100067138671875</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -1776,142 +1884,19 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
-        <v>43622</v>
+        <v>43805</v>
       </c>
       <c r="B67" s="3">
-        <v>43623</v>
+        <v>43808</v>
       </c>
       <c r="C67">
-        <v>-0.40999984741210938</v>
+        <v>0.4499969482421875</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="2">
-        <v>43644</v>
-      </c>
-      <c r="B68" s="3">
-        <v>43647</v>
-      </c>
-      <c r="C68">
-        <v>5.08001708984375</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="2">
-        <v>43658</v>
-      </c>
-      <c r="B69" s="3">
-        <v>43661</v>
-      </c>
-      <c r="C69">
-        <v>1.189994812011719</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="2">
-        <v>43685</v>
-      </c>
-      <c r="C70">
-        <v>7.3300018310546884</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="2">
-        <v>43728</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="2">
-        <v>43733</v>
-      </c>
-      <c r="B72" s="3">
-        <v>43734</v>
-      </c>
-      <c r="C72">
-        <v>51.6201171875</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="2">
-        <v>43740</v>
-      </c>
-      <c r="B73" s="3">
-        <v>43741</v>
-      </c>
-      <c r="C73">
-        <v>-0.70999908447265625</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="2">
-        <v>43789</v>
-      </c>
-      <c r="B74" s="3">
-        <v>43790</v>
-      </c>
-      <c r="C74">
-        <v>5.260009765625</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="2">
-        <v>43803</v>
-      </c>
-      <c r="C75">
-        <v>0.2100067138671875</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="2">
-        <v>43805</v>
-      </c>
-      <c r="B76" s="3">
-        <v>43808</v>
-      </c>
-      <c r="C76">
-        <v>0.4499969482421875</v>
       </c>
     </row>
   </sheetData>
@@ -1921,16 +1906,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="2" width="17.41796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
@@ -1959,16 +1939,25 @@
       <c r="C2">
         <v>-2.2700004577636719</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>42384</v>
       </c>
+      <c r="B3" s="3">
+        <v>42388</v>
+      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1978,11 +1967,14 @@
       <c r="A4" s="2">
         <v>42432</v>
       </c>
+      <c r="B4" s="3">
+        <v>42433</v>
+      </c>
       <c r="C4">
         <v>0.70833301544189453</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1990,10 +1982,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
-        <v>42433</v>
+        <v>42458</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42459</v>
+      </c>
+      <c r="C5">
+        <v>401.33984375</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2001,21 +1999,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
-        <v>42458</v>
+        <v>42475</v>
       </c>
       <c r="B6" s="3">
-        <v>42459</v>
+        <v>42478</v>
       </c>
       <c r="C6">
-        <v>401.33984375</v>
+        <v>-0.62999916076660156</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
-        <v>42467</v>
+        <v>42482</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42485</v>
+      </c>
+      <c r="C7">
+        <v>0.48999786376953119</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2023,16 +2033,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
-        <v>42475</v>
+        <v>42551</v>
       </c>
       <c r="B8" s="3">
-        <v>42478</v>
+        <v>42552</v>
       </c>
       <c r="C8">
-        <v>-0.62999916076660156</v>
+        <v>500</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2040,24 +2050,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
-        <v>42482</v>
+        <v>42615</v>
       </c>
       <c r="B9" s="3">
-        <v>42485</v>
+        <v>42619</v>
       </c>
       <c r="C9">
-        <v>0.48999786376953119</v>
+        <v>0.607330322265625</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
-        <v>42551</v>
+        <v>42620</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42621</v>
       </c>
       <c r="C10">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2065,10 +2084,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
-        <v>42615</v>
+        <v>42634</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42635</v>
       </c>
       <c r="C11">
-        <v>0.607330322265625</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2079,35 +2101,47 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
-        <v>42620</v>
+        <v>42642</v>
       </c>
       <c r="B12" s="3">
-        <v>42621</v>
+        <v>42643</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.6399993896484375</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
-        <v>42634</v>
+        <v>42705</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42706</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.26999855041503912</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
-        <v>42642</v>
+        <v>42794</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42795</v>
       </c>
       <c r="C14">
-        <v>0.6399993896484375</v>
+        <v>-0.34999942779541021</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2118,27 +2152,33 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
-        <v>42705</v>
+        <v>42795</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42796</v>
       </c>
       <c r="C15">
-        <v>0.26999855041503912</v>
+        <v>-0.82999992370605469</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
-        <v>42794</v>
+        <v>42809</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42810</v>
       </c>
       <c r="C16">
-        <v>-0.34999942779541021</v>
+        <v>47.83984375</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -2146,18 +2186,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
-        <v>42795</v>
+        <v>42828</v>
       </c>
       <c r="B17" s="3">
-        <v>42796</v>
+        <v>42829</v>
       </c>
       <c r="C17">
-        <v>-0.82999992370605469</v>
+        <v>-0.28000020980834961</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
-        <v>42804</v>
+        <v>42829</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42830</v>
+      </c>
+      <c r="C18">
+        <v>-1.920005798339844</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2168,38 +2220,50 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
-        <v>42809</v>
+        <v>42887</v>
       </c>
       <c r="B19" s="3">
-        <v>42810</v>
+        <v>42888</v>
       </c>
       <c r="C19">
-        <v>47.83984375</v>
+        <v>0.15640068054199219</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
-        <v>42828</v>
+        <v>42941</v>
+      </c>
+      <c r="B20" s="3">
+        <v>42942</v>
       </c>
       <c r="C20">
-        <v>-0.28000020980834961</v>
+        <v>1.1599998474121089</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
-        <v>42829</v>
+        <v>42954</v>
+      </c>
+      <c r="B21" s="3">
+        <v>42955</v>
       </c>
       <c r="C21">
-        <v>-1.920005798339844</v>
+        <v>0.6399993896484375</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2207,41 +2271,50 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
-        <v>42887</v>
+        <v>42978</v>
       </c>
       <c r="B22" s="3">
-        <v>42888</v>
+        <v>42979</v>
       </c>
       <c r="C22">
-        <v>0.15640068054199219</v>
+        <v>2.49072265625</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
-        <v>42941</v>
+        <v>43165</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43166</v>
       </c>
       <c r="C23">
-        <v>1.1599998474121089</v>
+        <v>-5.999755859375E-2</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
-        <v>42954</v>
+        <v>43193</v>
       </c>
       <c r="B24" s="3">
-        <v>42955</v>
+        <v>43194</v>
       </c>
       <c r="C24">
-        <v>0.6399993896484375</v>
+        <v>9.998321533203125E-3</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2249,21 +2322,33 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
-        <v>42978</v>
+        <v>43255</v>
       </c>
       <c r="B25" s="3">
-        <v>42979</v>
+        <v>43256</v>
       </c>
       <c r="C25">
-        <v>2.49072265625</v>
+        <v>6.999969482421875E-2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
-        <v>43102</v>
+        <v>43257</v>
+      </c>
+      <c r="B26" s="3">
+        <v>43258</v>
+      </c>
+      <c r="C26">
+        <v>1.999664306640625E-2</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -2271,46 +2356,67 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
-        <v>43165</v>
+        <v>43371</v>
       </c>
       <c r="B27" s="3">
-        <v>43166</v>
+        <v>43374</v>
       </c>
       <c r="C27">
-        <v>-5.999755859375E-2</v>
+        <v>-1.2899932861328121</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
-        <v>43175</v>
+        <v>43383</v>
+      </c>
+      <c r="B28" s="3">
+        <v>43384</v>
+      </c>
+      <c r="C28">
+        <v>1.000213623046875E-2</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
-        <v>43193</v>
+        <v>43409</v>
       </c>
       <c r="B29" s="3">
-        <v>43194</v>
+        <v>43410</v>
       </c>
       <c r="C29">
-        <v>9.998321533203125E-3</v>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
-        <v>43255</v>
+        <v>43416</v>
+      </c>
+      <c r="B30" s="3">
+        <v>43417</v>
       </c>
       <c r="C30">
-        <v>6.999969482421875E-2</v>
+        <v>-0.68589973449707031</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2318,43 +2424,64 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
-        <v>43257</v>
+        <v>43433</v>
       </c>
       <c r="B31" s="3">
-        <v>43258</v>
+        <v>43437</v>
       </c>
       <c r="C31">
-        <v>1.999664306640625E-2</v>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
-        <v>43356</v>
+        <v>43434</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43437</v>
+      </c>
+      <c r="C32">
+        <v>-5.8100013732910156</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
-        <v>43371</v>
+        <v>43465</v>
       </c>
       <c r="B33" s="3">
-        <v>43374</v>
+        <v>43467</v>
       </c>
       <c r="C33">
-        <v>-1.2899932861328121</v>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
-        <v>43383</v>
+        <v>43482</v>
+      </c>
+      <c r="B34" s="3">
+        <v>43483</v>
       </c>
       <c r="C34">
-        <v>1.000213623046875E-2</v>
+        <v>-0.67000007629394531</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2365,10 +2492,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
-        <v>43409</v>
+        <v>43509</v>
+      </c>
+      <c r="B35" s="3">
+        <v>43511</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.71999931335449219</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2379,13 +2509,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
-        <v>43416</v>
+        <v>43522</v>
       </c>
       <c r="B36" s="3">
-        <v>43417</v>
+        <v>43523</v>
       </c>
       <c r="C36">
-        <v>-0.68589973449707031</v>
+        <v>-0.28999900817871088</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2396,35 +2526,47 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
-        <v>43433</v>
+        <v>43556</v>
       </c>
       <c r="B37" s="3">
-        <v>43437</v>
+        <v>43557</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1.9500007629394529</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
-        <v>43434</v>
+        <v>43616</v>
+      </c>
+      <c r="B38" s="3">
+        <v>43619</v>
       </c>
       <c r="C38">
-        <v>-5.8100013732910156</v>
+        <v>-1.040000915527344</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
-        <v>43465</v>
+        <v>43622</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43623</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>-0.19999980926513669</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2435,13 +2577,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
-        <v>43482</v>
+        <v>43685</v>
+      </c>
+      <c r="B40" s="3">
+        <v>43686</v>
       </c>
       <c r="C40">
-        <v>-0.67000007629394531</v>
+        <v>0.1699981689453125</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2449,21 +2594,30 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
-        <v>43509</v>
+        <v>43733</v>
       </c>
       <c r="B41" s="3">
-        <v>43511</v>
+        <v>43734</v>
       </c>
       <c r="C41">
-        <v>0.71999931335449219</v>
+        <v>-0.13108634948730469</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
-        <v>43522</v>
+        <v>43740</v>
+      </c>
+      <c r="B42" s="3">
+        <v>43741</v>
       </c>
       <c r="C42">
-        <v>-0.28999900817871088</v>
+        <v>-1.100000381469727</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2474,10 +2628,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
-        <v>43556</v>
+        <v>43789</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43790</v>
       </c>
       <c r="C43">
-        <v>1.9500007629394529</v>
+        <v>0.1100006103515625</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2488,13 +2645,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
-        <v>43616</v>
+        <v>43803</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43804</v>
       </c>
       <c r="C44">
-        <v>-1.040000915527344</v>
+        <v>0.75</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2502,104 +2662,18 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
-        <v>43622</v>
+        <v>43805</v>
+      </c>
+      <c r="B45" s="3">
+        <v>43808</v>
       </c>
       <c r="C45">
-        <v>-0.19999980926513669</v>
+        <v>0.8699951171875</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2">
-        <v>43658</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2">
-        <v>43685</v>
-      </c>
-      <c r="B47" s="3">
-        <v>43686</v>
-      </c>
-      <c r="C47">
-        <v>0.1699981689453125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="2">
-        <v>43733</v>
-      </c>
-      <c r="C48">
-        <v>-0.13108634948730469</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="2">
-        <v>43740</v>
-      </c>
-      <c r="C49">
-        <v>-1.100000381469727</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="2">
-        <v>43789</v>
-      </c>
-      <c r="C50">
-        <v>0.1100006103515625</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2">
-        <v>43803</v>
-      </c>
-      <c r="B51" s="3">
-        <v>43804</v>
-      </c>
-      <c r="C51">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2">
-        <v>43805</v>
-      </c>
-      <c r="C52">
-        <v>0.8699951171875</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed total to percentage
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_analysis.xlsx
+++ b/sp500-historical-components-and-changes/sp500_analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003D5FC6-A8D0-482C-8E36-4000B696E457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="regular_add" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <sheet name="ad_hoc_delete" sheetId="4" r:id="rId4"/>
     <sheet name="population_stats" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -74,11 +68,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,14 +140,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -199,7 +186,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,27 +218,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,24 +252,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,14 +427,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>42811</v>
       </c>
@@ -508,7 +459,7 @@
         <v>42814</v>
       </c>
       <c r="C2">
-        <v>0.2299919128417969</v>
+        <v>-0.008209370913091929</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -517,7 +468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>42902</v>
       </c>
@@ -525,7 +476,7 @@
         <v>42905</v>
       </c>
       <c r="C3">
-        <v>4.9699935913085938</v>
+        <v>0.02144547179431167</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -534,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>42993</v>
       </c>
@@ -542,7 +493,7 @@
         <v>42996</v>
       </c>
       <c r="C4">
-        <v>0.25</v>
+        <v>0.006575486506837924</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -551,7 +502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43175</v>
       </c>
@@ -559,7 +510,7 @@
         <v>43178</v>
       </c>
       <c r="C5">
-        <v>3.4099960327148442</v>
+        <v>0.01043441828925395</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -568,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>43266</v>
       </c>
@@ -576,7 +527,7 @@
         <v>43269</v>
       </c>
       <c r="C6">
-        <v>-1.1699981689453121</v>
+        <v>-0.01348504562229558</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -585,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>43455</v>
       </c>
@@ -593,7 +544,7 @@
         <v>43458</v>
       </c>
       <c r="C7">
-        <v>-1.819999694824219</v>
+        <v>-0.02051628580326281</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -602,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>43728</v>
       </c>
@@ -610,7 +561,7 @@
         <v>43731</v>
       </c>
       <c r="C8">
-        <v>-0.7400054931640625</v>
+        <v>-0.006075578609383125</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -619,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>43819</v>
       </c>
@@ -627,7 +578,7 @@
         <v>43822</v>
       </c>
       <c r="C9">
-        <v>0.80999755859375</v>
+        <v>0.00724318476325525</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -642,14 +593,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -666,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>42811</v>
       </c>
@@ -674,7 +625,7 @@
         <v>42814</v>
       </c>
       <c r="C2">
-        <v>-0.35999870300292969</v>
+        <v>-0.01501871978787928</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -683,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>42902</v>
       </c>
@@ -691,7 +642,7 @@
         <v>42905</v>
       </c>
       <c r="C3">
-        <v>-7.9999923706054688E-2</v>
+        <v>-0.002818883934875172</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -700,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>43175</v>
       </c>
@@ -708,7 +659,7 @@
         <v>43178</v>
       </c>
       <c r="C4">
-        <v>0.64000034332275391</v>
+        <v>0.02165247000721815</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -717,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43266</v>
       </c>
@@ -734,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>43455</v>
       </c>
@@ -751,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>43819</v>
       </c>
@@ -759,7 +710,7 @@
         <v>43822</v>
       </c>
       <c r="C7">
-        <v>-1.0800018310546879</v>
+        <v>-0.03856507195478154</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -774,14 +725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -798,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>42373</v>
       </c>
@@ -806,7 +757,7 @@
         <v>42374</v>
       </c>
       <c r="C2">
-        <v>-3.6821136474609379</v>
+        <v>-0.02861844668334679</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -815,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>42384</v>
       </c>
@@ -823,7 +774,7 @@
         <v>42388</v>
       </c>
       <c r="C3">
-        <v>-1.19000244140625</v>
+        <v>-0.01364368751148082</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -832,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>42398</v>
       </c>
@@ -840,7 +791,7 @@
         <v>42401</v>
       </c>
       <c r="C4">
-        <v>2.5100002288818359</v>
+        <v>-0.002245507932528201</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -849,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>42419</v>
       </c>
@@ -857,7 +808,7 @@
         <v>42422</v>
       </c>
       <c r="C5">
-        <v>-1.6699981689453121</v>
+        <v>-0.01777350133266753</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -866,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>42432</v>
       </c>
@@ -874,7 +825,7 @@
         <v>42433</v>
       </c>
       <c r="C6">
-        <v>-0.8600006103515625</v>
+        <v>-0.01250728015754987</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -883,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>42433</v>
       </c>
@@ -891,7 +842,7 @@
         <v>42436</v>
       </c>
       <c r="C7">
-        <v>-1.7700004577636721</v>
+        <v>-0.04845334018370695</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -900,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>42458</v>
       </c>
@@ -908,7 +859,7 @@
         <v>42459</v>
       </c>
       <c r="C8">
-        <v>3.4999847412109382E-2</v>
+        <v>0.001341041133803067</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -917,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>42461</v>
       </c>
@@ -925,7 +876,7 @@
         <v>42464</v>
       </c>
       <c r="C9">
-        <v>-0.75</v>
+        <v>-0.01162790697674421</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -934,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>42467</v>
       </c>
@@ -942,7 +893,7 @@
         <v>42468</v>
       </c>
       <c r="C10">
-        <v>-0.238311767578125</v>
+        <v>-0.005741660039353058</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -951,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>42475</v>
       </c>
@@ -959,7 +910,7 @@
         <v>42478</v>
       </c>
       <c r="C11">
-        <v>-1.6100006103515621</v>
+        <v>-0.007828077136603273</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -968,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>42482</v>
       </c>
@@ -976,7 +927,7 @@
         <v>42485</v>
       </c>
       <c r="C12">
-        <v>-0.9799957275390625</v>
+        <v>-0.01319504203357935</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -985,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>42492</v>
       </c>
@@ -993,7 +944,7 @@
         <v>42493</v>
       </c>
       <c r="C13">
-        <v>1.3000030517578121</v>
+        <v>0.005330284370048677</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1002,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>42502</v>
       </c>
@@ -1010,7 +961,7 @@
         <v>42503</v>
       </c>
       <c r="C14">
-        <v>-2.029998779296875</v>
+        <v>-0.03002956841891069</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1019,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>42507</v>
       </c>
@@ -1027,7 +978,7 @@
         <v>42508</v>
       </c>
       <c r="C15">
-        <v>-1.8699951171875</v>
+        <v>-0.01922281188993469</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1036,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>42510</v>
       </c>
@@ -1044,7 +995,7 @@
         <v>42513</v>
       </c>
       <c r="C16">
-        <v>-3.9999008178710938E-2</v>
+        <v>-0.001271424327486836</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1053,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>42517</v>
       </c>
@@ -1061,7 +1012,7 @@
         <v>42521</v>
       </c>
       <c r="C17">
-        <v>0.19000244140625</v>
+        <v>0.003957559842717728</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1070,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>42523</v>
       </c>
@@ -1078,7 +1029,7 @@
         <v>42524</v>
       </c>
       <c r="C18">
-        <v>-0.25</v>
+        <v>-0.0009395317503125833</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1087,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>42542</v>
       </c>
@@ -1095,7 +1046,7 @@
         <v>42543</v>
       </c>
       <c r="C19">
-        <v>-6.999969482421875E-2</v>
+        <v>-0.00121442913888703</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1104,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>42551</v>
       </c>
@@ -1112,7 +1063,7 @@
         <v>42552</v>
       </c>
       <c r="C20">
-        <v>0.18999481201171881</v>
+        <v>0.002401349916787421</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1121,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>42615</v>
       </c>
@@ -1129,7 +1080,7 @@
         <v>42619</v>
       </c>
       <c r="C21">
-        <v>-3.170013427734375</v>
+        <v>-0.007832608762040616</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1138,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>42620</v>
       </c>
@@ -1146,7 +1097,7 @@
         <v>42621</v>
       </c>
       <c r="C22">
-        <v>2.889984130859375</v>
+        <v>0.01052165867978783</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1155,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>42634</v>
       </c>
@@ -1163,7 +1114,7 @@
         <v>42635</v>
       </c>
       <c r="C23">
-        <v>-0.230010986328125</v>
+        <v>-0.00123389829842524</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1172,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>42642</v>
       </c>
@@ -1180,7 +1131,7 @@
         <v>42643</v>
       </c>
       <c r="C24">
-        <v>-0.73999977111816406</v>
+        <v>-0.0310663216036462</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1189,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>42705</v>
       </c>
@@ -1197,7 +1148,7 @@
         <v>42706</v>
       </c>
       <c r="C25">
-        <v>-3.1491546630859379</v>
+        <v>-0.03595562178709522</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1206,7 +1157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>42739</v>
       </c>
@@ -1214,7 +1165,7 @@
         <v>42740</v>
       </c>
       <c r="C26">
-        <v>-1.650001525878906</v>
+        <v>-0.01403062540210831</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1223,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>42793</v>
       </c>
@@ -1231,7 +1182,7 @@
         <v>42794</v>
       </c>
       <c r="C27">
-        <v>2.80999755859375</v>
+        <v>0.02141603090320365</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1240,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>42794</v>
       </c>
@@ -1248,7 +1199,7 @@
         <v>42795</v>
       </c>
       <c r="C28">
-        <v>-0.90999603271484375</v>
+        <v>-0.01152477258442364</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1257,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>42795</v>
       </c>
@@ -1265,7 +1216,7 @@
         <v>42796</v>
       </c>
       <c r="C29">
-        <v>-1.9499969482421879</v>
+        <v>-0.02771850732817727</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1274,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>42804</v>
       </c>
@@ -1282,7 +1233,7 @@
         <v>42807</v>
       </c>
       <c r="C30">
-        <v>-1.459999084472656</v>
+        <v>-0.02298849193919184</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1291,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>42809</v>
       </c>
@@ -1299,7 +1250,7 @@
         <v>42810</v>
       </c>
       <c r="C31">
-        <v>-0.51000213623046875</v>
+        <v>-0.007207491815059419</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1308,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>42828</v>
       </c>
@@ -1316,7 +1267,7 @@
         <v>42829</v>
       </c>
       <c r="C32">
-        <v>-0.91695404052734375</v>
+        <v>-0.01536007651730231</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1325,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>42829</v>
       </c>
@@ -1333,7 +1284,7 @@
         <v>42830</v>
       </c>
       <c r="C33">
-        <v>-0.25</v>
+        <v>-0.002294630628753125</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1342,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>42887</v>
       </c>
@@ -1350,7 +1301,7 @@
         <v>42888</v>
       </c>
       <c r="C34">
-        <v>0.76000213623046875</v>
+        <v>0.01657583776495497</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1359,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>42941</v>
       </c>
@@ -1367,7 +1318,7 @@
         <v>42942</v>
       </c>
       <c r="C35">
-        <v>-0.86999893188476563</v>
+        <v>-0.01527534272020026</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1376,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>42954</v>
       </c>
@@ -1384,7 +1335,7 @@
         <v>42955</v>
       </c>
       <c r="C36">
-        <v>-2.8499984741210942</v>
+        <v>-0.04413812122643612</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1393,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>42978</v>
       </c>
@@ -1401,7 +1352,7 @@
         <v>42979</v>
       </c>
       <c r="C37">
-        <v>0.510009765625</v>
+        <v>0.003332526058541063</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1410,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>43020</v>
       </c>
@@ -1418,7 +1369,7 @@
         <v>43021</v>
       </c>
       <c r="C38">
-        <v>6.0001373291015618E-2</v>
+        <v>0.001020431531794985</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1427,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>43102</v>
       </c>
@@ -1435,7 +1386,7 @@
         <v>43103</v>
       </c>
       <c r="C39">
-        <v>-7.69000244140625</v>
+        <v>-0.03262623055143654</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1444,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>43165</v>
       </c>
@@ -1452,7 +1403,7 @@
         <v>43166</v>
       </c>
       <c r="C40">
-        <v>5.4600067138671884</v>
+        <v>0.02313758289991363</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1461,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>43193</v>
       </c>
@@ -1469,7 +1420,7 @@
         <v>43194</v>
       </c>
       <c r="C41">
-        <v>-0.2299957275390625</v>
+        <v>-0.001575960831105228</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1478,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>43250</v>
       </c>
@@ -1486,7 +1437,7 @@
         <v>43251</v>
       </c>
       <c r="C42">
-        <v>1.170013427734375</v>
+        <v>0.003020168936933354</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1495,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>43255</v>
       </c>
@@ -1503,7 +1454,7 @@
         <v>43256</v>
       </c>
       <c r="C43">
-        <v>-1.0800018310546879</v>
+        <v>-0.01960787572896872</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1512,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>43257</v>
       </c>
@@ -1520,7 +1471,7 @@
         <v>43258</v>
       </c>
       <c r="C44">
-        <v>0.29999923706054688</v>
+        <v>0.007537669417370108</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1529,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>43270</v>
       </c>
@@ -1537,7 +1488,7 @@
         <v>43271</v>
       </c>
       <c r="C45">
-        <v>-0.3600006103515625</v>
+        <v>-0.001633100192181547</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1546,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>43280</v>
       </c>
@@ -1554,7 +1505,7 @@
         <v>43283</v>
       </c>
       <c r="C46">
-        <v>0.5500030517578125</v>
+        <v>0.00981972983824142</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1563,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>43339</v>
       </c>
@@ -1571,7 +1522,7 @@
         <v>43340</v>
       </c>
       <c r="C47">
-        <v>-3.78997802734375</v>
+        <v>-0.01228199556764253</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1580,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>43356</v>
       </c>
@@ -1588,7 +1539,7 @@
         <v>43357</v>
       </c>
       <c r="C48">
-        <v>-3.660003662109375</v>
+        <v>-0.01199725824970932</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1597,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>43371</v>
       </c>
@@ -1605,7 +1556,7 @@
         <v>43374</v>
       </c>
       <c r="C49">
-        <v>0.95333099365234375</v>
+        <v>0.02413088827082976</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1614,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <v>43383</v>
       </c>
@@ -1622,7 +1573,7 @@
         <v>43384</v>
       </c>
       <c r="C50">
-        <v>-2.9899978637695308</v>
+        <v>-0.03621606046738912</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1631,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>43409</v>
       </c>
@@ -1639,7 +1590,7 @@
         <v>43410</v>
       </c>
       <c r="C51">
-        <v>1.1599998474121089</v>
+        <v>0.02028681079435235</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1648,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>43416</v>
       </c>
@@ -1656,7 +1607,7 @@
         <v>43417</v>
       </c>
       <c r="C52">
-        <v>-0.19000244140625</v>
+        <v>-0.0013427734375</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1665,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5">
       <c r="A53" s="2">
         <v>43434</v>
       </c>
@@ -1673,7 +1624,7 @@
         <v>43437</v>
       </c>
       <c r="C53">
-        <v>-1.0800056457519529</v>
+        <v>-0.004504933628032837</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1682,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5">
       <c r="A54" s="2">
         <v>43465</v>
       </c>
@@ -1690,7 +1641,7 @@
         <v>43467</v>
       </c>
       <c r="C54">
-        <v>-1.040000915527344</v>
+        <v>-0.01182625524965486</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1699,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5">
       <c r="A55" s="2">
         <v>43482</v>
       </c>
@@ -1707,7 +1658,7 @@
         <v>43483</v>
       </c>
       <c r="C55">
-        <v>6.05999755859375</v>
+        <v>0.02437257711337515</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1716,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5">
       <c r="A56" s="2">
         <v>43510</v>
       </c>
@@ -1724,7 +1675,7 @@
         <v>43511</v>
       </c>
       <c r="C56">
-        <v>-0.62999725341796875</v>
+        <v>-0.006522386140425107</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1733,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5">
       <c r="A57" s="2">
         <v>43522</v>
       </c>
@@ -1741,7 +1692,7 @@
         <v>43523</v>
       </c>
       <c r="C57">
-        <v>-4.0999984741210938</v>
+        <v>-0.05252368181338374</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1750,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5">
       <c r="A58" s="2">
         <v>43556</v>
       </c>
@@ -1758,7 +1709,7 @@
         <v>43557</v>
       </c>
       <c r="C58">
-        <v>1.8699989318847661</v>
+        <v>0.03621923093547275</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1767,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5">
       <c r="A59" s="2">
         <v>43616</v>
       </c>
@@ -1775,7 +1726,7 @@
         <v>43619</v>
       </c>
       <c r="C59">
-        <v>-1.8299999237060549</v>
+        <v>-0.06354166570085062</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1784,139 +1735,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5">
       <c r="A60" s="2">
+        <v>43622</v>
+      </c>
+      <c r="B60" s="3">
+        <v>43623</v>
+      </c>
+      <c r="C60">
+        <v>-0.007255350550167683</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2">
         <v>43644</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B61" s="3">
         <v>43647</v>
       </c>
-      <c r="C60">
-        <v>5.08001708984375</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="2">
+      <c r="C61">
+        <v>0.01605872525969709</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2">
         <v>43658</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B62" s="3">
         <v>43661</v>
       </c>
-      <c r="C61">
-        <v>1.189994812011719</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="2">
+      <c r="C62">
+        <v>0.01520565780128957</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2">
         <v>43685</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B63" s="3">
         <v>43686</v>
       </c>
-      <c r="C62">
-        <v>7.3300018310546884</v>
-      </c>
-      <c r="D62">
+      <c r="C63">
+        <v>0.06662778630923505</v>
+      </c>
+      <c r="D63">
         <v>2</v>
       </c>
-      <c r="E62">
+      <c r="E63">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="2">
+    <row r="64" spans="1:5">
+      <c r="A64" s="2">
         <v>43733</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B64" s="3">
         <v>43734</v>
       </c>
-      <c r="C63">
-        <v>51.6201171875</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="2">
+      <c r="C64">
+        <v>0.01465073846828435</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2">
         <v>43740</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B65" s="3">
         <v>43741</v>
       </c>
-      <c r="C64">
-        <v>-0.70999908447265625</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="2">
+      <c r="C65">
+        <v>-0.01241040195481069</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2">
         <v>43789</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B66" s="3">
         <v>43790</v>
       </c>
-      <c r="C65">
-        <v>5.260009765625</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="2">
+      <c r="C66">
+        <v>0.01893861147322085</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2">
         <v>43803</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B67" s="3">
         <v>43804</v>
       </c>
-      <c r="C66">
-        <v>0.2100067138671875</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="2">
+      <c r="C67">
+        <v>0.00308742611337065</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2">
         <v>43805</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B68" s="3">
         <v>43808</v>
       </c>
-      <c r="C67">
-        <v>0.4499969482421875</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67">
+      <c r="C68">
+        <v>0.002447497806746135</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
         <v>1</v>
       </c>
     </row>
@@ -1926,14 +1894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>42373</v>
       </c>
@@ -1958,7 +1926,7 @@
         <v>42374</v>
       </c>
       <c r="C2">
-        <v>-2.2700004577636719</v>
+        <v>-0.0620897257247377</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1967,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>42384</v>
       </c>
@@ -1984,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>42432</v>
       </c>
@@ -1992,7 +1960,7 @@
         <v>42433</v>
       </c>
       <c r="C4">
-        <v>0.70833301544189453</v>
+        <v>0.08994704957992306</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2001,7 +1969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>42458</v>
       </c>
@@ -2009,7 +1977,7 @@
         <v>42459</v>
       </c>
       <c r="C5">
-        <v>401.33984375</v>
+        <v>0.06818213867931</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2018,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>42475</v>
       </c>
@@ -2026,7 +1994,7 @@
         <v>42478</v>
       </c>
       <c r="C6">
-        <v>-0.62999916076660156</v>
+        <v>-0.01954698013386591</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2035,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>42482</v>
       </c>
@@ -2043,7 +2011,7 @@
         <v>42485</v>
       </c>
       <c r="C7">
-        <v>0.48999786376953119</v>
+        <v>0.01516551664942312</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2052,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>42551</v>
       </c>
@@ -2060,7 +2028,7 @@
         <v>42552</v>
       </c>
       <c r="C8">
-        <v>500</v>
+        <v>0.008064516129032251</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2069,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>42615</v>
       </c>
@@ -2077,7 +2045,7 @@
         <v>42619</v>
       </c>
       <c r="C9">
-        <v>0.607330322265625</v>
+        <v>0.01288603554165579</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2086,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>42620</v>
       </c>
@@ -2103,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>42634</v>
       </c>
@@ -2120,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>42642</v>
       </c>
@@ -2128,7 +2096,7 @@
         <v>42643</v>
       </c>
       <c r="C12">
-        <v>0.6399993896484375</v>
+        <v>0.03725258313619628</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2137,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>42705</v>
       </c>
@@ -2145,7 +2113,7 @@
         <v>42706</v>
       </c>
       <c r="C13">
-        <v>0.26999855041503912</v>
+        <v>0.008463904502939323</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2154,7 +2122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>42794</v>
       </c>
@@ -2162,7 +2130,7 @@
         <v>42795</v>
       </c>
       <c r="C14">
-        <v>-0.34999942779541021</v>
+        <v>-0.02501782941540653</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2171,7 +2139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>42795</v>
       </c>
@@ -2179,7 +2147,7 @@
         <v>42796</v>
       </c>
       <c r="C15">
-        <v>-0.82999992370605469</v>
+        <v>-0.0608058569158717</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2188,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>42809</v>
       </c>
@@ -2196,7 +2164,7 @@
         <v>42810</v>
       </c>
       <c r="C16">
-        <v>47.83984375</v>
+        <v>0.01457509765662035</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2205,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>42828</v>
       </c>
@@ -2213,7 +2181,7 @@
         <v>42829</v>
       </c>
       <c r="C17">
-        <v>-0.28000020980834961</v>
+        <v>-0.03427175118648995</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2222,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>42829</v>
       </c>
@@ -2230,7 +2198,7 @@
         <v>42830</v>
       </c>
       <c r="C18">
-        <v>-1.920005798339844</v>
+        <v>-0.01779265807785357</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2239,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>42887</v>
       </c>
@@ -2247,7 +2215,7 @@
         <v>42888</v>
       </c>
       <c r="C19">
-        <v>0.15640068054199219</v>
+        <v>0.01029385291310803</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2256,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>42941</v>
       </c>
@@ -2264,7 +2232,7 @@
         <v>42942</v>
       </c>
       <c r="C20">
-        <v>1.1599998474121089</v>
+        <v>0.0659708501071874</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2273,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>42954</v>
       </c>
@@ -2281,7 +2249,7 @@
         <v>42955</v>
       </c>
       <c r="C21">
-        <v>0.6399993896484375</v>
+        <v>0.01612089111710757</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2290,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>42978</v>
       </c>
@@ -2298,7 +2266,7 @@
         <v>42979</v>
       </c>
       <c r="C22">
-        <v>2.49072265625</v>
+        <v>0.02696456671711611</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2307,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>43165</v>
       </c>
@@ -2315,7 +2283,7 @@
         <v>43166</v>
       </c>
       <c r="C23">
-        <v>-5.999755859375E-2</v>
+        <v>-0.0006658996627062486</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2324,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>43193</v>
       </c>
@@ -2332,7 +2300,7 @@
         <v>43194</v>
       </c>
       <c r="C24">
-        <v>9.998321533203125E-3</v>
+        <v>0.0002425599523800948</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2341,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>43255</v>
       </c>
@@ -2349,7 +2317,7 @@
         <v>43256</v>
       </c>
       <c r="C25">
-        <v>6.999969482421875E-2</v>
+        <v>0.004895083488850149</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2358,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>43257</v>
       </c>
@@ -2366,7 +2334,7 @@
         <v>43258</v>
       </c>
       <c r="C26">
-        <v>1.999664306640625E-2</v>
+        <v>0.0001563092552074874</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2375,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>43371</v>
       </c>
@@ -2383,7 +2351,7 @@
         <v>43374</v>
       </c>
       <c r="C27">
-        <v>-1.2899932861328121</v>
+        <v>-0.008333828684572886</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2392,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>43383</v>
       </c>
@@ -2400,7 +2368,7 @@
         <v>43384</v>
       </c>
       <c r="C28">
-        <v>1.000213623046875E-2</v>
+        <v>0.0002175323255773076</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2409,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>43409</v>
       </c>
@@ -2426,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>43416</v>
       </c>
@@ -2434,7 +2402,7 @@
         <v>43417</v>
       </c>
       <c r="C30">
-        <v>-0.68589973449707031</v>
+        <v>-0.03509743295445455</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2443,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>43433</v>
       </c>
@@ -2460,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>43434</v>
       </c>
@@ -2468,7 +2436,7 @@
         <v>43437</v>
       </c>
       <c r="C32">
-        <v>-5.8100013732910156</v>
+        <v>-0.0876573401749976</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2477,7 +2445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>43465</v>
       </c>
@@ -2494,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>43482</v>
       </c>
@@ -2502,7 +2470,7 @@
         <v>43483</v>
       </c>
       <c r="C34">
-        <v>-0.67000007629394531</v>
+        <v>-0.09530584015618548</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2511,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>43509</v>
       </c>
@@ -2519,7 +2487,7 @@
         <v>43511</v>
       </c>
       <c r="C35">
-        <v>0.71999931335449219</v>
+        <v>0.04403665422359881</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2528,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>43522</v>
       </c>
@@ -2536,7 +2504,7 @@
         <v>43523</v>
       </c>
       <c r="C36">
-        <v>-0.28999900817871088</v>
+        <v>-0.01444218173707978</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2545,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>43556</v>
       </c>
@@ -2553,7 +2521,7 @@
         <v>43557</v>
       </c>
       <c r="C37">
-        <v>1.9500007629394529</v>
+        <v>0.05373383063501413</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2562,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>43616</v>
       </c>
@@ -2570,7 +2538,7 @@
         <v>43619</v>
       </c>
       <c r="C38">
-        <v>-1.040000915527344</v>
+        <v>-0.03616136673333326</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2579,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>43622</v>
       </c>
@@ -2587,7 +2555,7 @@
         <v>43623</v>
       </c>
       <c r="C39">
-        <v>-0.19999980926513669</v>
+        <v>-0.01819834517110164</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2596,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>43685</v>
       </c>
@@ -2604,7 +2572,7 @@
         <v>43686</v>
       </c>
       <c r="C40">
-        <v>0.1699981689453125</v>
+        <v>0.004212045747633342</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2613,7 +2581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>43733</v>
       </c>
@@ -2621,7 +2589,7 @@
         <v>43734</v>
       </c>
       <c r="C41">
-        <v>-0.13108634948730469</v>
+        <v>-0.007063583453822742</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2630,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>43740</v>
       </c>
@@ -2638,7 +2606,7 @@
         <v>43741</v>
       </c>
       <c r="C42">
-        <v>-1.100000381469727</v>
+        <v>-0.05968531542350586</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2647,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>43789</v>
       </c>
@@ -2655,7 +2623,7 @@
         <v>43790</v>
       </c>
       <c r="C43">
-        <v>0.1100006103515625</v>
+        <v>0.001017299668414573</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2664,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>43803</v>
       </c>
@@ -2672,7 +2640,7 @@
         <v>43804</v>
       </c>
       <c r="C44">
-        <v>0.75</v>
+        <v>0.03195568904738955</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2681,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>43805</v>
       </c>
@@ -2689,7 +2657,7 @@
         <v>43808</v>
       </c>
       <c r="C45">
-        <v>0.8699951171875</v>
+        <v>0.0125612920928917</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2704,19 +2672,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="12.734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2745,12 +2708,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5.9399757385253906</v>
+        <v>-0.002587719594374649</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -2759,30 +2722,30 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <v>0.37124848365783691</v>
+        <v>-0.0001617324746484156</v>
       </c>
       <c r="F2">
-        <v>2.327441585220769</v>
+        <v>0.0139934674660749</v>
       </c>
       <c r="G2">
-        <v>4.9699935913085938</v>
+        <v>0.02144547179431167</v>
       </c>
       <c r="H2">
-        <v>-1.819999694824219</v>
+        <v>-0.02051628580326281</v>
       </c>
       <c r="I2">
-        <v>2.5321309938061298</v>
+        <v>-0.1834729989033052</v>
       </c>
       <c r="J2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>-0.88000011444091797</v>
+        <v>-0.03475020567031784</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -2791,62 +2754,62 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>-9.7777790493435324E-2</v>
+        <v>-0.003861133963368648</v>
       </c>
       <c r="F3">
-        <v>0.56266095443979092</v>
+        <v>0.01994161219146801</v>
       </c>
       <c r="G3">
-        <v>0.64000034332275391</v>
+        <v>0.02165247000721815</v>
       </c>
       <c r="H3">
-        <v>-1.0800018310546879</v>
+        <v>-0.03856507195478154</v>
       </c>
       <c r="I3">
-        <v>-2.7586316272673348</v>
+        <v>-3.073653267657873</v>
       </c>
       <c r="J3">
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.4444444444444444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <v>34.871963500976563</v>
+        <v>-0.3753668345492384</v>
       </c>
       <c r="C4">
         <v>27</v>
       </c>
       <c r="D4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E4">
-        <v>0.47124275001319682</v>
+        <v>-0.005004891127323178</v>
       </c>
       <c r="F4">
-        <v>6.8482396854887222</v>
+        <v>0.02136211753332594</v>
       </c>
       <c r="G4">
-        <v>51.6201171875</v>
+        <v>0.06662778630923505</v>
       </c>
       <c r="H4">
-        <v>-7.69000244140625</v>
+        <v>-0.06354166570085062</v>
       </c>
       <c r="I4">
-        <v>1.092360531409865</v>
+        <v>-3.719209177047119</v>
       </c>
       <c r="J4">
-        <v>0.36486486486486491</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5">
-        <v>943.46547651290894</v>
+        <v>-0.055220636439409</v>
       </c>
       <c r="C5">
         <v>31</v>
@@ -2855,22 +2818,22 @@
         <v>48</v>
       </c>
       <c r="E5">
-        <v>19.6555307606856</v>
+        <v>-0.001150429925821021</v>
       </c>
       <c r="F5">
-        <v>95.624790590488388</v>
+        <v>0.03731584316650061</v>
       </c>
       <c r="G5">
-        <v>500</v>
+        <v>0.08994704957992306</v>
       </c>
       <c r="H5">
-        <v>-5.8100013732910156</v>
+        <v>-0.09530584015618548</v>
       </c>
       <c r="I5">
-        <v>3.2629810298330959</v>
+        <v>-0.4894036247737303</v>
       </c>
       <c r="J5">
-        <v>0.64583333333333337</v>
+        <v>0.6458333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new output. regular add has problems
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_analysis.xlsx
+++ b/sp500-historical-components-and-changes/sp500_analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="22">
   <si>
     <t>eff_date</t>
   </si>
@@ -442,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>42373</v>
+        <v>42374</v>
       </c>
       <c r="C2" s="2">
         <v>42374</v>
@@ -512,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="J2">
-        <v>-0.0620897257247377</v>
+        <v>-0.02653834421450951</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>42384</v>
+        <v>42388</v>
       </c>
       <c r="C3" s="2">
         <v>42388</v>
@@ -550,10 +550,10 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <v>-0.01364368751148082</v>
+        <v>0.02871092939382369</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -564,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>42398</v>
+        <v>42401</v>
       </c>
       <c r="C4" s="2">
         <v>42401</v>
@@ -588,7 +588,7 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <v>0.02029358021268579</v>
+        <v>0.00762443733026319</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>42419</v>
+        <v>42422</v>
       </c>
       <c r="C5" s="2">
         <v>42422</v>
@@ -626,10 +626,10 @@
         <v>15</v>
       </c>
       <c r="J5">
-        <v>-0.01777350133266753</v>
+        <v>0.02903890214096738</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -640,16 +640,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>42432</v>
+        <v>42411</v>
       </c>
       <c r="C6" s="2">
-        <v>42433</v>
+        <v>42422</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -664,10 +664,10 @@
         <v>15</v>
       </c>
       <c r="J6">
-        <v>-0.01250728015754987</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -681,7 +681,7 @@
         <v>42433</v>
       </c>
       <c r="C7" s="2">
-        <v>42436</v>
+        <v>42433</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -702,7 +702,7 @@
         <v>15</v>
       </c>
       <c r="J7">
-        <v>-0.04845334018370695</v>
+        <v>-0.0004418082271389068</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -716,16 +716,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>42458</v>
+        <v>42436</v>
       </c>
       <c r="C8" s="2">
-        <v>42459</v>
+        <v>42436</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -740,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="J8">
-        <v>0.06818213867931</v>
+        <v>0.03107024980451878</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -754,16 +754,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>42461</v>
+        <v>42459</v>
       </c>
       <c r="C9" s="2">
-        <v>42464</v>
+        <v>42459</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -778,10 +778,10 @@
         <v>15</v>
       </c>
       <c r="J9">
-        <v>-0.01162790697674421</v>
+        <v>0.06382851497383024</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -792,10 +792,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>42467</v>
+        <v>42464</v>
       </c>
       <c r="C10" s="2">
-        <v>42468</v>
+        <v>42464</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -816,7 +816,7 @@
         <v>15</v>
       </c>
       <c r="J10">
-        <v>-0.005741660039353058</v>
+        <v>-0.003764732211243849</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -830,16 +830,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>42475</v>
+        <v>42468</v>
       </c>
       <c r="C11" s="2">
-        <v>42478</v>
+        <v>42468</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -854,10 +854,10 @@
         <v>15</v>
       </c>
       <c r="J11">
-        <v>-0.01954698013386591</v>
+        <v>0.05919150527292238</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -868,10 +868,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>42482</v>
+        <v>42478</v>
       </c>
       <c r="C12" s="2">
-        <v>42485</v>
+        <v>42478</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -892,7 +892,7 @@
         <v>15</v>
       </c>
       <c r="J12">
-        <v>0.01516551664942312</v>
+        <v>0.008544318180514932</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -906,16 +906,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>42492</v>
+        <v>42485</v>
       </c>
       <c r="C13" s="2">
-        <v>42493</v>
+        <v>42485</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -930,7 +930,7 @@
         <v>15</v>
       </c>
       <c r="J13">
-        <v>0.005330284370048677</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -944,10 +944,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>42502</v>
+        <v>42493</v>
       </c>
       <c r="C14" s="2">
-        <v>42503</v>
+        <v>42493</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -968,7 +968,7 @@
         <v>15</v>
       </c>
       <c r="J14">
-        <v>-0.03002956841891069</v>
+        <v>-0.01178677499438041</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -982,10 +982,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>42507</v>
+        <v>42503</v>
       </c>
       <c r="C15" s="2">
-        <v>42508</v>
+        <v>42503</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1006,10 +1006,10 @@
         <v>15</v>
       </c>
       <c r="J15">
-        <v>-0.01922281188993469</v>
+        <v>0.01052314236110496</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1020,10 +1020,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>42510</v>
+        <v>42508</v>
       </c>
       <c r="C16" s="2">
-        <v>42513</v>
+        <v>42508</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1044,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="J16">
-        <v>-0.001271424327486836</v>
+        <v>-0.01939006427530754</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1058,10 +1058,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>42517</v>
+        <v>42513</v>
       </c>
       <c r="C17" s="2">
-        <v>42521</v>
+        <v>42513</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1082,7 +1082,7 @@
         <v>15</v>
       </c>
       <c r="J17">
-        <v>0.003957559842717728</v>
+        <v>0.01527687909200504</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1096,10 +1096,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>42523</v>
+        <v>42521</v>
       </c>
       <c r="C18" s="2">
-        <v>42524</v>
+        <v>42521</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1120,10 +1120,10 @@
         <v>15</v>
       </c>
       <c r="J18">
-        <v>-0.0009395317503125833</v>
+        <v>0.002697117553060124</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -1134,10 +1134,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>42542</v>
+        <v>42524</v>
       </c>
       <c r="C19" s="2">
-        <v>42543</v>
+        <v>42524</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="J19">
-        <v>-0.00121442913888703</v>
+        <v>-0.005491993210917867</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1172,10 +1172,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>42551</v>
+        <v>42543</v>
       </c>
       <c r="C20" s="2">
-        <v>42552</v>
+        <v>42543</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1196,10 +1196,10 @@
         <v>15</v>
       </c>
       <c r="J20">
-        <v>-0.003013534224119097</v>
+        <v>-0.007121762195336112</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -1210,10 +1210,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>42615</v>
+        <v>42552</v>
       </c>
       <c r="C21" s="2">
-        <v>42619</v>
+        <v>42552</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1234,10 +1234,10 @@
         <v>15</v>
       </c>
       <c r="J21">
-        <v>-0.007832608762040616</v>
+        <v>0.01738031771911475</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1248,16 +1248,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>42620</v>
+        <v>42619</v>
       </c>
       <c r="C22" s="2">
-        <v>42621</v>
+        <v>42619</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>-1</v>
@@ -1272,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>0.008118565221587826</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -1286,16 +1286,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>42634</v>
+        <v>42621</v>
       </c>
       <c r="C23" s="2">
-        <v>42635</v>
+        <v>42621</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23">
         <v>-1</v>
@@ -1310,7 +1310,7 @@
         <v>15</v>
       </c>
       <c r="J23">
-        <v>-0.00123389829842524</v>
+        <v>-0.03333841234878154</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1324,10 +1324,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>42642</v>
+        <v>42635</v>
       </c>
       <c r="C24" s="2">
-        <v>42643</v>
+        <v>42635</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1348,7 +1348,7 @@
         <v>15</v>
       </c>
       <c r="J24">
-        <v>-0.0310663216036462</v>
+        <v>-0.009023486635896694</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1362,10 +1362,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>42705</v>
+        <v>42643</v>
       </c>
       <c r="C25" s="2">
-        <v>42706</v>
+        <v>42643</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1386,13 +1386,13 @@
         <v>15</v>
       </c>
       <c r="J25">
-        <v>-0.006161931845265256</v>
+        <v>0.01819757702263036</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1400,10 +1400,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>42739</v>
+        <v>42706</v>
       </c>
       <c r="C26" s="2">
-        <v>42740</v>
+        <v>42706</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1424,13 +1424,13 @@
         <v>15</v>
       </c>
       <c r="J26">
-        <v>-0.01403062540210831</v>
+        <v>0.03409838174627411</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1438,10 +1438,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>42793</v>
+        <v>42740</v>
       </c>
       <c r="C27" s="2">
-        <v>42794</v>
+        <v>42740</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1462,7 +1462,7 @@
         <v>15</v>
       </c>
       <c r="J27">
-        <v>0.02141603090320365</v>
+        <v>8.626249671173092E-05</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -1479,7 +1479,7 @@
         <v>42794</v>
       </c>
       <c r="C28" s="2">
-        <v>42795</v>
+        <v>42794</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1500,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="J28">
-        <v>-0.01152477258442364</v>
+        <v>-0.00686463318621422</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1517,13 +1517,13 @@
         <v>42795</v>
       </c>
       <c r="C29" s="2">
-        <v>42796</v>
+        <v>42795</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29">
         <v>-1</v>
@@ -1538,10 +1538,10 @@
         <v>15</v>
       </c>
       <c r="J29">
-        <v>-0.0608058569158717</v>
+        <v>0.01601537413356757</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -1552,16 +1552,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>42804</v>
+        <v>42796</v>
       </c>
       <c r="C30" s="2">
-        <v>42807</v>
+        <v>42796</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30">
         <v>-1</v>
@@ -1576,7 +1576,7 @@
         <v>15</v>
       </c>
       <c r="J30">
-        <v>-0.02298849193919184</v>
+        <v>-0.04134163382119005</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1590,16 +1590,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>42809</v>
+        <v>42807</v>
       </c>
       <c r="C31" s="2">
-        <v>42810</v>
+        <v>42807</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31">
         <v>-1</v>
@@ -1614,10 +1614,10 @@
         <v>15</v>
       </c>
       <c r="J31">
-        <v>0.01457509765662035</v>
+        <v>-0.00112811757751663</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -1628,13 +1628,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>42811</v>
+        <v>42810</v>
       </c>
       <c r="C32" s="2">
-        <v>42814</v>
+        <v>42810</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -1652,7 +1652,7 @@
         <v>15</v>
       </c>
       <c r="J32">
-        <v>-0.03486960686756557</v>
+        <v>-0.005747474038787947</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -1666,16 +1666,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <v>42828</v>
+        <v>42814</v>
       </c>
       <c r="C33" s="2">
-        <v>42829</v>
+        <v>42814</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33">
         <v>-1</v>
@@ -1690,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="J33">
-        <v>-0.01536007651730231</v>
+        <v>-0.0468111773386608</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1707,7 +1707,7 @@
         <v>42829</v>
       </c>
       <c r="C34" s="2">
-        <v>42830</v>
+        <v>42829</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -1728,10 +1728,10 @@
         <v>15</v>
       </c>
       <c r="J34">
-        <v>-0.002294630628753125</v>
+        <v>0.02133923018630091</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -1742,16 +1742,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="2">
-        <v>42887</v>
+        <v>42830</v>
       </c>
       <c r="C35" s="2">
-        <v>42888</v>
+        <v>42830</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F35">
         <v>-1</v>
@@ -1766,7 +1766,7 @@
         <v>15</v>
       </c>
       <c r="J35">
-        <v>0.01029385291310803</v>
+        <v>0.004875864062294122</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -1780,13 +1780,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="2">
-        <v>42902</v>
+        <v>42888</v>
       </c>
       <c r="C36" s="2">
-        <v>42905</v>
+        <v>42888</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1804,7 +1804,7 @@
         <v>15</v>
       </c>
       <c r="J36">
-        <v>-0.008709718873584182</v>
+        <v>-0.04364821235462368</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -1818,16 +1818,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="2">
-        <v>42941</v>
+        <v>42905</v>
       </c>
       <c r="C37" s="2">
-        <v>42942</v>
+        <v>42905</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37">
         <v>-1</v>
@@ -1842,13 +1842,13 @@
         <v>15</v>
       </c>
       <c r="J37">
-        <v>0.006347944659562454</v>
+        <v>0.014892032424074</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1856,16 +1856,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="2">
-        <v>42954</v>
+        <v>42942</v>
       </c>
       <c r="C38" s="2">
-        <v>42955</v>
+        <v>42942</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38">
         <v>-1</v>
@@ -1880,13 +1880,13 @@
         <v>15</v>
       </c>
       <c r="J38">
-        <v>0.01612089111710757</v>
+        <v>-0.0002574233134378101</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1894,10 +1894,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="2">
-        <v>42978</v>
+        <v>42955</v>
       </c>
       <c r="C39" s="2">
-        <v>42979</v>
+        <v>42955</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -1918,10 +1918,10 @@
         <v>15</v>
       </c>
       <c r="J39">
-        <v>0.02696456671711611</v>
+        <v>-0.008428362699599012</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -1932,16 +1932,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="2">
-        <v>42993</v>
+        <v>42979</v>
       </c>
       <c r="C40" s="2">
-        <v>42996</v>
+        <v>42979</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F40">
         <v>-1</v>
@@ -1956,7 +1956,7 @@
         <v>15</v>
       </c>
       <c r="J40">
-        <v>0.006575486506837924</v>
+        <v>0.007951993354786913</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -1970,10 +1970,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="2">
-        <v>43020</v>
+        <v>42996</v>
       </c>
       <c r="C41" s="2">
-        <v>43021</v>
+        <v>42996</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -1994,7 +1994,7 @@
         <v>15</v>
       </c>
       <c r="J41">
-        <v>0.001020431531794985</v>
+        <v>0.01332632128123579</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -2008,10 +2008,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>43102</v>
+        <v>43021</v>
       </c>
       <c r="C42" s="2">
-        <v>43103</v>
+        <v>43021</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2032,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="J42">
-        <v>-0.03262623055143654</v>
+        <v>-0.002038717815841529</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -2046,16 +2046,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2">
-        <v>43165</v>
+        <v>43103</v>
       </c>
       <c r="C43" s="2">
-        <v>43166</v>
+        <v>43103</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F43">
         <v>-1</v>
@@ -2070,10 +2070,10 @@
         <v>15</v>
       </c>
       <c r="J43">
-        <v>-0.0006658996627062486</v>
+        <v>0.006052387685010485</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -2084,13 +2084,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="2">
-        <v>43175</v>
+        <v>43166</v>
       </c>
       <c r="C44" s="2">
-        <v>43178</v>
+        <v>43166</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -2108,13 +2108,13 @@
         <v>15</v>
       </c>
       <c r="J44">
-        <v>0.01324502056478671</v>
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2122,10 +2122,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="2">
-        <v>43193</v>
+        <v>43178</v>
       </c>
       <c r="C45" s="2">
-        <v>43194</v>
+        <v>43178</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2146,13 +2146,13 @@
         <v>15</v>
       </c>
       <c r="J45">
-        <v>0.0002425599523800948</v>
+        <v>-0.0163398540036791</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2160,16 +2160,16 @@
         <v>44</v>
       </c>
       <c r="B46" s="2">
-        <v>43250</v>
+        <v>43193</v>
       </c>
       <c r="C46" s="2">
-        <v>43251</v>
+        <v>43194</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F46">
         <v>-1</v>
@@ -2184,7 +2184,7 @@
         <v>15</v>
       </c>
       <c r="J46">
-        <v>0.003020168936933354</v>
+        <v>0.0002425599523800948</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -2198,10 +2198,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="2">
-        <v>43255</v>
+        <v>43194</v>
       </c>
       <c r="C47" s="2">
-        <v>43256</v>
+        <v>43194</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -2222,10 +2222,10 @@
         <v>15</v>
       </c>
       <c r="J47">
-        <v>-0.01960787572896872</v>
+        <v>0.006794250145901515</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47">
         <v>1</v>
@@ -2236,16 +2236,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="2">
-        <v>43257</v>
+        <v>43251</v>
       </c>
       <c r="C48" s="2">
-        <v>43258</v>
+        <v>43251</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F48">
         <v>-1</v>
@@ -2260,10 +2260,10 @@
         <v>15</v>
       </c>
       <c r="J48">
-        <v>0.0001563092552074874</v>
+        <v>-0.01912137461907026</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -2274,16 +2274,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="2">
-        <v>43266</v>
+        <v>43256</v>
       </c>
       <c r="C49" s="2">
-        <v>43269</v>
+        <v>43256</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49">
         <v>-1</v>
@@ -2298,7 +2298,7 @@
         <v>15</v>
       </c>
       <c r="J49">
-        <v>-0.01052632076219306</v>
+        <v>0.004629629629629539</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -2312,16 +2312,16 @@
         <v>48</v>
       </c>
       <c r="B50" s="2">
-        <v>43270</v>
+        <v>43257</v>
       </c>
       <c r="C50" s="2">
-        <v>43271</v>
+        <v>43258</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50">
         <v>-1</v>
@@ -2336,10 +2336,10 @@
         <v>15</v>
       </c>
       <c r="J50">
-        <v>-0.001633100192181547</v>
+        <v>0.0001563092552074874</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>1</v>
@@ -2350,10 +2350,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="2">
-        <v>43280</v>
+        <v>43258</v>
       </c>
       <c r="C51" s="2">
-        <v>43283</v>
+        <v>43258</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -2374,10 +2374,10 @@
         <v>15</v>
       </c>
       <c r="J51">
-        <v>0.00981972983824142</v>
+        <v>-0.009975005645942447</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51">
         <v>1</v>
@@ -2388,16 +2388,16 @@
         <v>50</v>
       </c>
       <c r="B52" s="2">
-        <v>43339</v>
+        <v>43269</v>
       </c>
       <c r="C52" s="2">
-        <v>43340</v>
+        <v>43269</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52">
         <v>-1</v>
@@ -2412,13 +2412,13 @@
         <v>15</v>
       </c>
       <c r="J52">
-        <v>-0.01228199556764253</v>
+        <v>0.02440558874649956</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2426,16 +2426,16 @@
         <v>51</v>
       </c>
       <c r="B53" s="2">
-        <v>43356</v>
+        <v>43266</v>
       </c>
       <c r="C53" s="2">
-        <v>43357</v>
+        <v>43271</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F53">
         <v>-1</v>
@@ -2450,10 +2450,10 @@
         <v>15</v>
       </c>
       <c r="J53">
-        <v>-0.01199725824970932</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53">
         <v>1</v>
@@ -2464,16 +2464,16 @@
         <v>52</v>
       </c>
       <c r="B54" s="2">
-        <v>43371</v>
+        <v>43271</v>
       </c>
       <c r="C54" s="2">
-        <v>43374</v>
+        <v>43271</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F54">
         <v>-1</v>
@@ -2488,10 +2488,10 @@
         <v>15</v>
       </c>
       <c r="J54">
-        <v>-0.008333828684572886</v>
+        <v>0.007451832860794871</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54">
         <v>1</v>
@@ -2502,10 +2502,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="2">
-        <v>43383</v>
+        <v>43283</v>
       </c>
       <c r="C55" s="2">
-        <v>43384</v>
+        <v>43283</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -2526,10 +2526,10 @@
         <v>15</v>
       </c>
       <c r="J55">
-        <v>-0.03621606046738912</v>
+        <v>0.004950473346860607</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55">
         <v>1</v>
@@ -2540,10 +2540,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="2">
-        <v>43409</v>
+        <v>43340</v>
       </c>
       <c r="C56" s="2">
-        <v>43410</v>
+        <v>43340</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -2564,10 +2564,10 @@
         <v>15</v>
       </c>
       <c r="J56">
-        <v>0.02028681079435235</v>
+        <v>-0.00193574697775456</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56">
         <v>1</v>
@@ -2578,16 +2578,16 @@
         <v>55</v>
       </c>
       <c r="B57" s="2">
-        <v>43416</v>
+        <v>43357</v>
       </c>
       <c r="C57" s="2">
-        <v>43417</v>
+        <v>43357</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F57">
         <v>-1</v>
@@ -2602,10 +2602,10 @@
         <v>15</v>
       </c>
       <c r="J57">
-        <v>-0.03509743295445455</v>
+        <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L57">
         <v>1</v>
@@ -2616,10 +2616,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="2">
-        <v>43433</v>
+        <v>43374</v>
       </c>
       <c r="C58" s="2">
-        <v>43437</v>
+        <v>43374</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -2654,10 +2654,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="2">
-        <v>43434</v>
+        <v>43384</v>
       </c>
       <c r="C59" s="2">
-        <v>43437</v>
+        <v>43384</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2678,13 +2678,13 @@
         <v>15</v>
       </c>
       <c r="J59">
-        <v>-0.000521252497274638</v>
+        <v>-0.03079046069672853</v>
       </c>
       <c r="K59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -2692,16 +2692,16 @@
         <v>58</v>
       </c>
       <c r="B60" s="2">
-        <v>43455</v>
+        <v>43410</v>
       </c>
       <c r="C60" s="2">
-        <v>43458</v>
+        <v>43410</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F60">
         <v>-1</v>
@@ -2716,7 +2716,7 @@
         <v>15</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>0.006170733791737826</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -2730,16 +2730,16 @@
         <v>59</v>
       </c>
       <c r="B61" s="2">
-        <v>43465</v>
+        <v>43417</v>
       </c>
       <c r="C61" s="2">
-        <v>43467</v>
+        <v>43417</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F61">
         <v>-1</v>
@@ -2754,7 +2754,7 @@
         <v>15</v>
       </c>
       <c r="J61">
-        <v>-0.01182625524965486</v>
+        <v>-0.01574140504577448</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -2768,16 +2768,16 @@
         <v>60</v>
       </c>
       <c r="B62" s="2">
-        <v>43482</v>
+        <v>43433</v>
       </c>
       <c r="C62" s="2">
-        <v>43483</v>
+        <v>43437</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F62">
         <v>-1</v>
@@ -2792,7 +2792,7 @@
         <v>15</v>
       </c>
       <c r="J62">
-        <v>0.02437257711337515</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -2806,16 +2806,16 @@
         <v>61</v>
       </c>
       <c r="B63" s="2">
-        <v>43509</v>
+        <v>43437</v>
       </c>
       <c r="C63" s="2">
-        <v>43511</v>
+        <v>43437</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F63">
         <v>-1</v>
@@ -2830,13 +2830,13 @@
         <v>15</v>
       </c>
       <c r="J63">
-        <v>0.04403665422359881</v>
+        <v>-0.01460228372555583</v>
       </c>
       <c r="K63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L63">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -2844,16 +2844,16 @@
         <v>62</v>
       </c>
       <c r="B64" s="2">
-        <v>43510</v>
+        <v>43455</v>
       </c>
       <c r="C64" s="2">
-        <v>43511</v>
+        <v>43458</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F64">
         <v>-1</v>
@@ -2868,10 +2868,10 @@
         <v>15</v>
       </c>
       <c r="J64">
-        <v>-0.006522386140425107</v>
+        <v>0</v>
       </c>
       <c r="K64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64">
         <v>1</v>
@@ -2882,10 +2882,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="2">
-        <v>43522</v>
+        <v>43458</v>
       </c>
       <c r="C65" s="2">
-        <v>43523</v>
+        <v>43458</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
@@ -2906,7 +2906,7 @@
         <v>15</v>
       </c>
       <c r="J65">
-        <v>-0.05252368181338374</v>
+        <v>-0.02796639800028911</v>
       </c>
       <c r="K65">
         <v>0</v>
@@ -2920,10 +2920,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="2">
-        <v>43556</v>
+        <v>43467</v>
       </c>
       <c r="C66" s="2">
-        <v>43557</v>
+        <v>43467</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -2944,7 +2944,7 @@
         <v>15</v>
       </c>
       <c r="J66">
-        <v>0.03621923093547275</v>
+        <v>0.00690447023688967</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -2958,10 +2958,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="2">
-        <v>43616</v>
+        <v>43483</v>
       </c>
       <c r="C67" s="2">
-        <v>43619</v>
+        <v>43483</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
@@ -2982,10 +2982,10 @@
         <v>15</v>
       </c>
       <c r="J67">
-        <v>-0.06354166570085062</v>
+        <v>0.0126423891561589</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L67">
         <v>1</v>
@@ -2996,16 +2996,16 @@
         <v>66</v>
       </c>
       <c r="B68" s="2">
-        <v>43622</v>
+        <v>43509</v>
       </c>
       <c r="C68" s="2">
-        <v>43623</v>
+        <v>43511</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F68">
         <v>-1</v>
@@ -3020,10 +3020,10 @@
         <v>15</v>
       </c>
       <c r="J68">
-        <v>-0.007255350550167683</v>
+        <v>0.04403665422359881</v>
       </c>
       <c r="K68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L68">
         <v>1</v>
@@ -3034,10 +3034,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="2">
-        <v>43644</v>
+        <v>43511</v>
       </c>
       <c r="C69" s="2">
-        <v>43647</v>
+        <v>43511</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -3058,7 +3058,7 @@
         <v>15</v>
       </c>
       <c r="J69">
-        <v>0.01605872525969709</v>
+        <v>0.01135894099296131</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -3072,10 +3072,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="2">
-        <v>43658</v>
+        <v>43523</v>
       </c>
       <c r="C70" s="2">
-        <v>43661</v>
+        <v>43523</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -3096,7 +3096,7 @@
         <v>15</v>
       </c>
       <c r="J70">
-        <v>0.01520565780128957</v>
+        <v>0.01811795543364836</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -3110,16 +3110,16 @@
         <v>69</v>
       </c>
       <c r="B71" s="2">
-        <v>43685</v>
+        <v>43557</v>
       </c>
       <c r="C71" s="2">
-        <v>43686</v>
+        <v>43557</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F71">
         <v>-1</v>
@@ -3134,7 +3134,7 @@
         <v>15</v>
       </c>
       <c r="J71">
-        <v>0.004212045747633342</v>
+        <v>0.05140186915887845</v>
       </c>
       <c r="K71">
         <v>1</v>
@@ -3148,13 +3148,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="2">
-        <v>43728</v>
+        <v>43619</v>
       </c>
       <c r="C72" s="2">
-        <v>43731</v>
+        <v>43619</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
@@ -3172,7 +3172,7 @@
         <v>15</v>
       </c>
       <c r="J72">
-        <v>-0.006075578609383125</v>
+        <v>-0.08008898414552656</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -3186,16 +3186,16 @@
         <v>71</v>
       </c>
       <c r="B73" s="2">
-        <v>43733</v>
+        <v>43623</v>
       </c>
       <c r="C73" s="2">
-        <v>43734</v>
+        <v>43623</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73">
         <v>-1</v>
@@ -3210,7 +3210,7 @@
         <v>15</v>
       </c>
       <c r="J73">
-        <v>0.01465073846828435</v>
+        <v>0.007414265429924516</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -3224,10 +3224,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="2">
-        <v>43740</v>
+        <v>43647</v>
       </c>
       <c r="C74" s="2">
-        <v>43741</v>
+        <v>43647</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -3248,10 +3248,10 @@
         <v>15</v>
       </c>
       <c r="J74">
-        <v>-0.01241040195481069</v>
+        <v>0.003608901425150579</v>
       </c>
       <c r="K74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74">
         <v>1</v>
@@ -3262,10 +3262,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="2">
-        <v>43789</v>
+        <v>43661</v>
       </c>
       <c r="C75" s="2">
-        <v>43790</v>
+        <v>43661</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -3286,10 +3286,10 @@
         <v>15</v>
       </c>
       <c r="J75">
-        <v>0.01893861147322085</v>
+        <v>-0.00176210692291956</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75">
         <v>1</v>
@@ -3300,10 +3300,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="2">
-        <v>43803</v>
+        <v>43686</v>
       </c>
       <c r="C76" s="2">
-        <v>43804</v>
+        <v>43686</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
@@ -3324,7 +3324,7 @@
         <v>15</v>
       </c>
       <c r="J76">
-        <v>0.03195568904738955</v>
+        <v>0.009622487081042186</v>
       </c>
       <c r="K76">
         <v>1</v>
@@ -3338,10 +3338,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="2">
-        <v>43805</v>
+        <v>43731</v>
       </c>
       <c r="C77" s="2">
-        <v>43808</v>
+        <v>43731</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
@@ -3362,10 +3362,10 @@
         <v>15</v>
       </c>
       <c r="J77">
-        <v>0.002447539302419477</v>
+        <v>-0.01420784119767249</v>
       </c>
       <c r="K77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L77">
         <v>1</v>
@@ -3376,36 +3376,302 @@
         <v>76</v>
       </c>
       <c r="B78" s="2">
-        <v>43819</v>
+        <v>43734</v>
       </c>
       <c r="C78" s="2">
+        <v>43734</v>
+      </c>
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78">
+        <v>-1</v>
+      </c>
+      <c r="G78" t="s">
+        <v>15</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>15</v>
+      </c>
+      <c r="J78">
+        <v>0.01032725087412589</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="2">
+        <v>43741</v>
+      </c>
+      <c r="C79" s="2">
+        <v>43741</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79">
+        <v>-1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>15</v>
+      </c>
+      <c r="J79">
+        <v>-0.009734499770983174</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2">
+        <v>43790</v>
+      </c>
+      <c r="C80" s="2">
+        <v>43790</v>
+      </c>
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80">
+        <v>-1</v>
+      </c>
+      <c r="G80" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>15</v>
+      </c>
+      <c r="J80">
+        <v>-0.01371026460357772</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2">
+        <v>43803</v>
+      </c>
+      <c r="C81" s="2">
+        <v>43804</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81">
+        <v>-1</v>
+      </c>
+      <c r="G81" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>15</v>
+      </c>
+      <c r="J81">
+        <v>0.03195568904738955</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2">
+        <v>43804</v>
+      </c>
+      <c r="C82" s="2">
+        <v>43804</v>
+      </c>
+      <c r="D82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82">
+        <v>-1</v>
+      </c>
+      <c r="G82" t="s">
+        <v>15</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
+        <v>15</v>
+      </c>
+      <c r="J82">
+        <v>0.02169127443533481</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2">
+        <v>43808</v>
+      </c>
+      <c r="C83" s="2">
+        <v>43808</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83">
+        <v>-1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>15</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>15</v>
+      </c>
+      <c r="J83">
+        <v>0.01383536080834236</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2">
+        <v>43805</v>
+      </c>
+      <c r="C84" s="2">
+        <v>43808</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84">
+        <v>-1</v>
+      </c>
+      <c r="G84" t="s">
+        <v>15</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>15</v>
+      </c>
+      <c r="J84">
+        <v>0.0125612920928917</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2">
         <v>43822</v>
       </c>
-      <c r="D78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="C85" s="2">
+        <v>43822</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" t="s">
         <v>13</v>
       </c>
-      <c r="F78">
-        <v>-1</v>
-      </c>
-      <c r="G78" t="s">
-        <v>15</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78" t="s">
-        <v>15</v>
-      </c>
-      <c r="J78">
-        <v>-0.02526245679698158</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
+      <c r="F85">
+        <v>-1</v>
+      </c>
+      <c r="G85" t="s">
+        <v>15</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>15</v>
+      </c>
+      <c r="J85">
+        <v>0.01455625274477623</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
         <v>2</v>
       </c>
     </row>
@@ -3416,7 +3682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3492,31 +3758,31 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>-0.06612308273553769</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K2">
-        <v>-0.007347009192837521</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.01724797995621445</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0.01324502056478671</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>-0.03486960686756557</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>-6.761960271417113</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.4444444444444444</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3524,10 +3790,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>-1</v>
@@ -3542,31 +3808,31 @@
         <v>15</v>
       </c>
       <c r="H3">
-        <v>0.0004999078974547988</v>
+        <v>0.002233081641310086</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="K3">
-        <v>0.0002499539487273994</v>
+        <v>7.203489165516407E-05</v>
       </c>
       <c r="L3">
-        <v>0.008945653932912483</v>
+        <v>0.0253782313635978</v>
       </c>
       <c r="M3">
-        <v>0.006575486506837924</v>
+        <v>0.06382851497383024</v>
       </c>
       <c r="N3">
-        <v>-0.006075578609383125</v>
+        <v>-0.0468111773386608</v>
       </c>
       <c r="O3">
-        <v>0.4435557148828674</v>
+        <v>0.04505902865534296</v>
       </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>0.6129032258064516</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3577,7 +3843,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>-1</v>
@@ -3592,81 +3858,31 @@
         <v>15</v>
       </c>
       <c r="H4">
-        <v>0.04536559788268546</v>
+        <v>0.2123042968505561</v>
       </c>
       <c r="I4">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="J4">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="K4">
-        <v>0.002387663046457129</v>
+        <v>0.00348039830902551</v>
       </c>
       <c r="L4">
-        <v>0.03187681257828975</v>
+        <v>0.02057999259891393</v>
       </c>
       <c r="M4">
-        <v>0.06818213867931</v>
+        <v>0.05919150527292238</v>
       </c>
       <c r="N4">
-        <v>-0.0620897257247377</v>
+        <v>-0.08008898414552656</v>
       </c>
       <c r="O4">
-        <v>1.189045351387517</v>
+        <v>2.684627317975957</v>
       </c>
       <c r="P4">
-        <v>0.6842105263157895</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>-0.3275099267529054</v>
-      </c>
-      <c r="I5">
-        <v>17</v>
-      </c>
-      <c r="J5">
-        <v>56</v>
-      </c>
-      <c r="K5">
-        <v>-0.005848391549159024</v>
-      </c>
-      <c r="L5">
-        <v>0.01977920333980824</v>
-      </c>
-      <c r="M5">
-        <v>0.03621923093547275</v>
-      </c>
-      <c r="N5">
-        <v>-0.06354166570085062</v>
-      </c>
-      <c r="O5">
-        <v>-4.693836048795051</v>
-      </c>
-      <c r="P5">
-        <v>0.3035714285714285</v>
+        <v>0.6229508196721312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>